<commit_message>
Make BOMs parse-able by Kitspace
</commit_message>
<xml_diff>
--- a/PCB/BOM/SHIELD_008.xlsx
+++ b/PCB/BOM/SHIELD_008.xlsx
@@ -33,7 +33,7 @@
     <t xml:space="preserve">SHIELD_008</t>
   </si>
   <si>
-    <t xml:space="preserve">part</t>
+    <t xml:space="preserve">References</t>
   </si>
   <si>
     <t xml:space="preserve">pcs/pcb</t>
@@ -480,7 +480,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -521,10 +521,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -545,10 +541,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -558,10 +550,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -607,15 +595,15 @@
   </sheetPr>
   <dimension ref="B1:H23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.01171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.42"/>
@@ -663,14 +651,14 @@
       <c r="D3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="11"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="8" t="s">
@@ -682,133 +670,133 @@
       <c r="D4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="11"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>24</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="14" t="s">
+      <c r="G7" s="11"/>
+      <c r="H7" s="13" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="12"/>
-      <c r="H8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="12"/>
-      <c r="H9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>38</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="12"/>
-      <c r="H10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="12" t="s">
         <v>41</v>
       </c>
       <c r="C11" s="8" t="s">
@@ -817,17 +805,17 @@
       <c r="D11" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="9" t="s">
@@ -836,237 +824,237 @@
       <c r="D12" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="12"/>
-      <c r="H12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>45</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="14" t="s">
+      <c r="G13" s="11"/>
+      <c r="H13" s="13" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>49</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="12"/>
-      <c r="H14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="12" t="s">
         <v>53</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="14" t="s">
+      <c r="G15" s="11"/>
+      <c r="H15" s="13" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="12" t="s">
         <v>57</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="G16" s="12"/>
-      <c r="H16" s="14" t="s">
+      <c r="G16" s="11"/>
+      <c r="H16" s="13" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="12" t="s">
         <v>61</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="G17" s="12"/>
-      <c r="H17" s="14" t="s">
+      <c r="G17" s="11"/>
+      <c r="H17" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="12" t="s">
         <v>65</v>
       </c>
       <c r="C18" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G18" s="12"/>
-      <c r="H18" s="14" t="s">
+      <c r="G18" s="11"/>
+      <c r="H18" s="13" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="12" t="s">
         <v>69</v>
       </c>
       <c r="C19" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="G19" s="12"/>
-      <c r="H19" s="14" t="s">
+      <c r="G19" s="11"/>
+      <c r="H19" s="13" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="14" t="s">
         <v>74</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11" t="s">
+      <c r="E20" s="10"/>
+      <c r="F20" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="G20" s="12"/>
-      <c r="H20" s="14" t="s">
+      <c r="G20" s="11"/>
+      <c r="H20" s="13" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="E21" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="F21" s="21" t="s">
+      <c r="F21" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="G21" s="22"/>
-      <c r="H21" s="14" t="s">
+      <c r="G21" s="19"/>
+      <c r="H21" s="13" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="13" t="n">
+      <c r="C22" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="G22" s="23"/>
-      <c r="H22" s="24" t="s">
+      <c r="G22" s="20"/>
+      <c r="H22" s="21" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C23" s="11" t="n">
+      <c r="C23" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="11" t="n">
+      <c r="D23" s="20"/>
+      <c r="E23" s="10" t="n">
         <v>68710614522</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G23" s="23"/>
-      <c r="H23" s="14" t="s">
+      <c r="G23" s="20"/>
+      <c r="H23" s="13" t="s">
         <v>87</v>
       </c>
     </row>

</xml_diff>